<commit_message>
rerun with update OR calculation
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -454,7 +454,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.598140185981402</v>
+        <v>0.597740225977402</v>
       </c>
     </row>
     <row r="4">
@@ -487,7 +487,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0690930906909309</v>
+        <v>0.0693930606939306</v>
       </c>
     </row>
     <row r="7">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.223977602239776</v>
+        <v>0.222277772222778</v>
       </c>
     </row>
     <row r="8">
@@ -509,7 +509,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.779122087791221</v>
+        <v>0.777722227777222</v>
       </c>
     </row>
     <row r="9">
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.42045795420458</v>
+        <v>0.407959204079592</v>
       </c>
     </row>
     <row r="4">
@@ -611,7 +611,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.272972702729727</v>
+        <v>0.265673432656734</v>
       </c>
     </row>
     <row r="7">
@@ -622,7 +622,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.288871112888711</v>
+        <v>0.279372062793721</v>
       </c>
     </row>
     <row r="8">
@@ -633,7 +633,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.952804719528047</v>
+        <v>0.965603439656034</v>
       </c>
     </row>
     <row r="9">
@@ -655,7 +655,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>0.257120459926824</v>
+        <v>0.743616658580255</v>
       </c>
     </row>
   </sheetData>
@@ -702,7 +702,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.61963803619638</v>
+        <v>0.619338066193381</v>
       </c>
     </row>
     <row r="4">
@@ -735,7 +735,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0157984201579842</v>
+        <v>0.0140985901409859</v>
       </c>
     </row>
     <row r="7">
@@ -746,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.771922807719228</v>
+        <v>0.771822817718228</v>
       </c>
     </row>
     <row r="8">
@@ -815,7 +815,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.365963403659634</v>
+        <v>0.368463153684632</v>
       </c>
     </row>
     <row r="4">
@@ -837,7 +837,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0006999300069993</v>
+        <v>0.0000999900009999</v>
       </c>
     </row>
     <row r="6">
@@ -848,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.490850914908509</v>
+        <v>0.497750224977502</v>
       </c>
     </row>
     <row r="7">
@@ -859,7 +859,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.283071692830717</v>
+        <v>0.273272672732727</v>
       </c>
     </row>
     <row r="8">
@@ -870,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.167883211678832</v>
+        <v>0.170882911708829</v>
       </c>
     </row>
     <row r="9">
@@ -939,7 +939,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.568943105689431</v>
+        <v>0.564243575642436</v>
       </c>
     </row>
     <row r="4">
@@ -972,7 +972,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.803719628037196</v>
+        <v>0.794620537946205</v>
       </c>
     </row>
     <row r="7">
@@ -983,7 +983,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0104989501049895</v>
+        <v>0.0115988401159884</v>
       </c>
     </row>
     <row r="8">
@@ -994,7 +994,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.658034196580342</v>
+        <v>0.652134786521348</v>
       </c>
     </row>
     <row r="9">
@@ -1063,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.942105789421058</v>
+        <v>0.942705729427057</v>
       </c>
     </row>
     <row r="4">
@@ -1085,7 +1085,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0005999400059994</v>
+        <v>0.0003999600039996</v>
       </c>
     </row>
     <row r="6">
@@ -1096,7 +1096,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.686231376862314</v>
+        <v>0.688131186881312</v>
       </c>
     </row>
     <row r="7">
@@ -1107,7 +1107,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.311868813118688</v>
+        <v>0.314768523147685</v>
       </c>
     </row>
     <row r="8">
@@ -1187,7 +1187,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0003999600039996</v>
+        <v>0.0002999700029997</v>
       </c>
     </row>
     <row r="5">
@@ -1198,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.14998500149985</v>
+        <v>0.148585141485851</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0552944705529447</v>
+        <v>0.0556944305569443</v>
       </c>
     </row>
     <row r="7">
@@ -1220,7 +1220,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.306169383061694</v>
+        <v>0.298870112988701</v>
       </c>
     </row>
     <row r="8">
@@ -1289,7 +1289,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.190580941905809</v>
+        <v>0.196880311968803</v>
       </c>
     </row>
     <row r="4">
@@ -1300,7 +1300,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0001999800019998</v>
+        <v>0.0002999700029997</v>
       </c>
     </row>
     <row r="5">
@@ -1311,7 +1311,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.479152084791521</v>
+        <v>0.488851114888511</v>
       </c>
     </row>
     <row r="6">
@@ -1333,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.376562343765623</v>
+        <v>0.391860813918608</v>
       </c>
     </row>
     <row r="8">
@@ -1402,7 +1402,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.911308869113089</v>
+        <v>0.917008299170083</v>
       </c>
     </row>
     <row r="4">
@@ -1435,7 +1435,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.244375562443756</v>
+        <v>0.256374362563744</v>
       </c>
     </row>
     <row r="7">
@@ -1446,7 +1446,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.857714228577142</v>
+        <v>0.853814618538146</v>
       </c>
     </row>
     <row r="8">
@@ -1515,7 +1515,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.187081291870813</v>
+        <v>0.192680731926807</v>
       </c>
     </row>
     <row r="4">
@@ -1548,7 +1548,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.526947305269473</v>
+        <v>0.524647535246475</v>
       </c>
     </row>
     <row r="7">
@@ -1559,7 +1559,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.794520547945205</v>
+        <v>0.788721127887211</v>
       </c>
     </row>
     <row r="8">
@@ -1570,7 +1570,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.697030296970303</v>
+        <v>0.704729527047295</v>
       </c>
     </row>
     <row r="9">
@@ -1639,7 +1639,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.784221577842216</v>
+        <v>0.784921507849215</v>
       </c>
     </row>
     <row r="4">
@@ -1672,7 +1672,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.48005199480052</v>
+        <v>0.473252674732527</v>
       </c>
     </row>
     <row r="7">
@@ -1683,7 +1683,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2997700229977</v>
+        <v>0.299170082991701</v>
       </c>
     </row>
     <row r="8">
@@ -1694,7 +1694,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.685831416858314</v>
+        <v>0.68043195680432</v>
       </c>
     </row>
     <row r="9">
@@ -1763,7 +1763,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.810818918108189</v>
+        <v>0.800619938006199</v>
       </c>
     </row>
     <row r="4">
@@ -1785,7 +1785,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.502049795020498</v>
+        <v>0.503649635036496</v>
       </c>
     </row>
     <row r="6">
@@ -1796,7 +1796,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.934606539346065</v>
+        <v>0.931806819318068</v>
       </c>
     </row>
     <row r="7">
@@ -1807,7 +1807,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.851014898510149</v>
+        <v>0.848715128487151</v>
       </c>
     </row>
     <row r="8">
@@ -1876,7 +1876,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.123187681231877</v>
+        <v>0.126687331266873</v>
       </c>
     </row>
     <row r="4">
@@ -1898,7 +1898,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0002999700029997</v>
+        <v>0.0000999900009999</v>
       </c>
     </row>
     <row r="6">
@@ -1909,7 +1909,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.020997900209979</v>
+        <v>0.0238976102389761</v>
       </c>
     </row>
     <row r="7">
@@ -1920,7 +1920,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.853514648535146</v>
+        <v>0.842215778422158</v>
       </c>
     </row>
     <row r="8">
@@ -1931,7 +1931,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.481351864813519</v>
+        <v>0.487851214878512</v>
       </c>
     </row>
     <row r="9">
@@ -2000,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.614838516148385</v>
+        <v>0.61973802619738</v>
       </c>
     </row>
     <row r="4">
@@ -2011,7 +2011,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0002999700029997</v>
+        <v>0.0000999900009999</v>
       </c>
     </row>
     <row r="5">
@@ -2022,7 +2022,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0090990900909909</v>
+        <v>0.00999900009999</v>
       </c>
     </row>
     <row r="6">
@@ -2033,7 +2033,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.858614138586141</v>
+        <v>0.855014498550145</v>
       </c>
     </row>
     <row r="7">
@@ -2044,7 +2044,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.354064593540646</v>
+        <v>0.361363863613639</v>
       </c>
     </row>
     <row r="8">
@@ -2055,7 +2055,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.277572242775722</v>
+        <v>0.275772422757724</v>
       </c>
     </row>
     <row r="9">
@@ -2124,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.73962603739626</v>
+        <v>0.739526047395261</v>
       </c>
     </row>
     <row r="4">
@@ -2146,7 +2146,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0053994600539946</v>
+        <v>0.0045995400459954</v>
       </c>
     </row>
     <row r="6">
@@ -2157,7 +2157,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.166883311668833</v>
+        <v>0.165783421657834</v>
       </c>
     </row>
     <row r="7">
@@ -2168,7 +2168,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.571242875712429</v>
+        <v>0.582741725827417</v>
       </c>
     </row>
     <row r="8">
@@ -2237,7 +2237,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0533946605339466</v>
+        <v>0.044995500449955</v>
       </c>
     </row>
     <row r="4">
@@ -2259,7 +2259,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0005999400059994</v>
+        <v>0.0002999700029997</v>
       </c>
     </row>
     <row r="6">
@@ -2270,7 +2270,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.881711828817118</v>
+        <v>0.875612438756124</v>
       </c>
     </row>
     <row r="7">
@@ -2281,7 +2281,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.992900709929007</v>
+        <v>0.992600739926007</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
replace derived cell lines with solid tumors
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -454,7 +454,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.602539746025398</v>
+        <v>0.603839616038396</v>
       </c>
     </row>
     <row r="4">
@@ -487,7 +487,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0716928307169283</v>
+        <v>0.0754924507549245</v>
       </c>
     </row>
     <row r="7">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.231876812318768</v>
+        <v>0.218878112188781</v>
       </c>
     </row>
     <row r="8">
@@ -509,7 +509,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.776722327767223</v>
+        <v>0.789421057894211</v>
       </c>
     </row>
     <row r="9">
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.394860513948605</v>
+        <v>0.388761123887611</v>
       </c>
     </row>
     <row r="4">
@@ -611,7 +611,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.258674132586741</v>
+        <v>0.256674332566743</v>
       </c>
     </row>
     <row r="7">
@@ -622,7 +622,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.286771322867713</v>
+        <v>0.285171482851715</v>
       </c>
     </row>
     <row r="8">
@@ -633,7 +633,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.965803419658034</v>
+        <v>0.967303269673033</v>
       </c>
     </row>
     <row r="9">
@@ -702,7 +702,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.625037496250375</v>
+        <v>0.615538446155384</v>
       </c>
     </row>
     <row r="4">
@@ -735,7 +735,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0177982201779822</v>
+        <v>0.0173982601739826</v>
       </c>
     </row>
     <row r="7">
@@ -746,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.768923107689231</v>
+        <v>0.768523147685231</v>
       </c>
     </row>
     <row r="8">
@@ -848,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.506449355064494</v>
+        <v>0.4997500249975</v>
       </c>
     </row>
     <row r="7">
@@ -859,7 +859,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.275472452754725</v>
+        <v>0.275772422757724</v>
       </c>
     </row>
     <row r="8">
@@ -870,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.168783121687831</v>
+        <v>0.173682631736826</v>
       </c>
     </row>
     <row r="9">
@@ -939,7 +939,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.56974302569743</v>
+        <v>0.565043495650435</v>
       </c>
     </row>
     <row r="4">
@@ -972,7 +972,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.795720427957204</v>
+        <v>0.8001199880012</v>
       </c>
     </row>
     <row r="7">
@@ -994,7 +994,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.65973402659734</v>
+        <v>0.655634436556344</v>
       </c>
     </row>
     <row r="9">
@@ -1063,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.947405259474053</v>
+        <v>0.946905309469053</v>
       </c>
     </row>
     <row r="4">
@@ -1096,7 +1096,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.68973102689731</v>
+        <v>0.689431056894311</v>
       </c>
     </row>
     <row r="7">
@@ -1107,7 +1107,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.317768223177682</v>
+        <v>0.318368163183682</v>
       </c>
     </row>
     <row r="8">
@@ -1187,7 +1187,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0002999700029997</v>
+        <v>0.0003999600039996</v>
       </c>
     </row>
     <row r="5">
@@ -1198,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.155584441555844</v>
+        <v>0.154284571542846</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0597940205979402</v>
+        <v>0.0600939906009399</v>
       </c>
     </row>
     <row r="7">
@@ -1220,7 +1220,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.304569543045695</v>
+        <v>0.292170782921708</v>
       </c>
     </row>
     <row r="8">
@@ -1289,7 +1289,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.195280471952805</v>
+        <v>0.195880411958804</v>
       </c>
     </row>
     <row r="4">
@@ -1300,7 +1300,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0004999500049995</v>
+        <v>0.0007999200079992</v>
       </c>
     </row>
     <row r="5">
@@ -1311,7 +1311,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.487451254874513</v>
+        <v>0.478752124787521</v>
       </c>
     </row>
     <row r="6">
@@ -1333,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.371062893710629</v>
+        <v>0.388561143885611</v>
       </c>
     </row>
     <row r="8">
@@ -1402,7 +1402,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.912808719128087</v>
+        <v>0.916808319168083</v>
       </c>
     </row>
     <row r="4">
@@ -1424,7 +1424,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0000999900009999</v>
+        <v>0.0001999800019998</v>
       </c>
     </row>
     <row r="6">
@@ -1435,7 +1435,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.259074092590741</v>
+        <v>0.255874412558744</v>
       </c>
     </row>
     <row r="7">
@@ -1446,7 +1446,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.853814618538146</v>
+        <v>0.855414458554145</v>
       </c>
     </row>
     <row r="8">
@@ -1515,7 +1515,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.193680631936806</v>
+        <v>0.194980501949805</v>
       </c>
     </row>
     <row r="4">
@@ -1548,7 +1548,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.515848415158484</v>
+        <v>0.526747325267473</v>
       </c>
     </row>
     <row r="7">
@@ -1559,7 +1559,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.79012098790121</v>
+        <v>0.788321167883212</v>
       </c>
     </row>
     <row r="8">
@@ -1570,7 +1570,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.701929807019298</v>
+        <v>0.695630436956304</v>
       </c>
     </row>
     <row r="9">
@@ -1639,7 +1639,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.777122287771223</v>
+        <v>0.783721627837216</v>
       </c>
     </row>
     <row r="4">
@@ -1672,7 +1672,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.480751924807519</v>
+        <v>0.465753424657534</v>
       </c>
     </row>
     <row r="7">
@@ -1683,7 +1683,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.290970902909709</v>
+        <v>0.295770422957704</v>
       </c>
     </row>
     <row r="8">
@@ -1694,7 +1694,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.68033196680332</v>
+        <v>0.674632536746325</v>
       </c>
     </row>
     <row r="9">
@@ -1763,7 +1763,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.806519348065193</v>
+        <v>0.805919408059194</v>
       </c>
     </row>
     <row r="4">
@@ -1785,7 +1785,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.504649535046495</v>
+        <v>0.503049695030497</v>
       </c>
     </row>
     <row r="6">
@@ -1796,7 +1796,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.932206779322068</v>
+        <v>0.935206479352065</v>
       </c>
     </row>
     <row r="7">
@@ -1807,7 +1807,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.846815318468153</v>
+        <v>0.846415358464154</v>
       </c>
     </row>
     <row r="8">
@@ -1876,7 +1876,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.130586941305869</v>
+        <v>0.121687831216878</v>
       </c>
     </row>
     <row r="4">
@@ -1898,7 +1898,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0003999600039996</v>
+        <v>0.0001999800019998</v>
       </c>
     </row>
     <row r="6">
@@ -1909,7 +1909,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0235976402359764</v>
+        <v>0.0223977602239776</v>
       </c>
     </row>
     <row r="7">
@@ -1920,7 +1920,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.85041495850415</v>
+        <v>0.849315068493151</v>
       </c>
     </row>
     <row r="8">
@@ -1931,7 +1931,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.47965203479652</v>
+        <v>0.488151184881512</v>
       </c>
     </row>
     <row r="9">
@@ -2000,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.618238176182382</v>
+        <v>0.610838916108389</v>
       </c>
     </row>
     <row r="4">
@@ -2011,7 +2011,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0000999900009999</v>
+        <v>0.0002999700029997</v>
       </c>
     </row>
     <row r="5">
@@ -2022,7 +2022,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0108989101089891</v>
+        <v>0.0077992200779922</v>
       </c>
     </row>
     <row r="6">
@@ -2033,7 +2033,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.855714428557144</v>
+        <v>0.853914608539146</v>
       </c>
     </row>
     <row r="7">
@@ -2044,7 +2044,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.362263773622638</v>
+        <v>0.352564743525647</v>
       </c>
     </row>
     <row r="8">
@@ -2055,7 +2055,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.276472352764724</v>
+        <v>0.283271672832717</v>
       </c>
     </row>
     <row r="9">
@@ -2124,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.734226577342266</v>
+        <v>0.733826617338266</v>
       </c>
     </row>
     <row r="4">
@@ -2146,7 +2146,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0055994400559944</v>
+        <v>0.004999500049995</v>
       </c>
     </row>
     <row r="6">
@@ -2157,7 +2157,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.165683431656834</v>
+        <v>0.163983601639836</v>
       </c>
     </row>
     <row r="7">
@@ -2168,7 +2168,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.584241575842416</v>
+        <v>0.581041895810419</v>
       </c>
     </row>
     <row r="8">
@@ -2237,7 +2237,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0442955704429557</v>
+        <v>0.0472952704729527</v>
       </c>
     </row>
     <row r="4">
@@ -2259,7 +2259,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0003999600039996</v>
+        <v>0.0006999300069993</v>
       </c>
     </row>
     <row r="6">
@@ -2270,7 +2270,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.875712428757124</v>
+        <v>0.879212078792121</v>
       </c>
     </row>
     <row r="7">
@@ -2281,7 +2281,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.992900709929007</v>
+        <v>0.994100589941006</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
rm derived cell line only samples
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -454,7 +454,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.603839616038396</v>
+        <v>0.609339066093391</v>
       </c>
     </row>
     <row r="4">
@@ -487,7 +487,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0754924507549245</v>
+        <v>0.0625937406259374</v>
       </c>
     </row>
     <row r="7">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.218878112188781</v>
+        <v>0.224777522247775</v>
       </c>
     </row>
     <row r="8">
@@ -509,7 +509,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.789421057894211</v>
+        <v>0.776322367763224</v>
       </c>
     </row>
     <row r="9">
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.388761123887611</v>
+        <v>0.406659334066593</v>
       </c>
     </row>
     <row r="4">
@@ -611,7 +611,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.256674332566743</v>
+        <v>0.264073592640736</v>
       </c>
     </row>
     <row r="7">
@@ -622,7 +622,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.285171482851715</v>
+        <v>0.280571942805719</v>
       </c>
     </row>
     <row r="8">
@@ -633,7 +633,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.967303269673033</v>
+        <v>0.965103489651035</v>
       </c>
     </row>
     <row r="9">
@@ -691,7 +691,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.652232662013525</v>
+        <v>0.579588377492154</v>
       </c>
     </row>
     <row r="3">
@@ -702,7 +702,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.615538446155384</v>
+        <v>0.618138186181382</v>
       </c>
     </row>
     <row r="4">
@@ -735,7 +735,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0173982601739826</v>
+        <v>0.0143985601439856</v>
       </c>
     </row>
     <row r="7">
@@ -746,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.768523147685231</v>
+        <v>0.764823517648235</v>
       </c>
     </row>
     <row r="8">
@@ -757,7 +757,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="n">
-        <v>0.124845238053223</v>
+        <v>0.111213887506894</v>
       </c>
     </row>
     <row r="9">
@@ -768,7 +768,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>0.259262165005025</v>
+        <v>0.239428006470177</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +815,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.37016298370163</v>
+        <v>0.367963203679632</v>
       </c>
     </row>
     <row r="4">
@@ -848,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4997500249975</v>
+        <v>0.558444155584442</v>
       </c>
     </row>
     <row r="7">
@@ -859,7 +859,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.275772422757724</v>
+        <v>0.279172082791721</v>
       </c>
     </row>
     <row r="8">
@@ -870,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.173682631736826</v>
+        <v>0.172282771722828</v>
       </c>
     </row>
     <row r="9">
@@ -928,7 +928,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.957322984148866</v>
+        <v>0.967518506841397</v>
       </c>
     </row>
     <row r="3">
@@ -939,7 +939,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.565043495650435</v>
+        <v>0.585041495850415</v>
       </c>
     </row>
     <row r="4">
@@ -972,7 +972,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8001199880012</v>
+        <v>0.890810918908109</v>
       </c>
     </row>
     <row r="7">
@@ -983,7 +983,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0104989501049895</v>
+        <v>0.0096990300969903</v>
       </c>
     </row>
     <row r="8">
@@ -994,7 +994,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.655634436556344</v>
+        <v>0.64043595640436</v>
       </c>
     </row>
     <row r="9">
@@ -1005,7 +1005,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.415013092936939</v>
+        <v>0.420853921755544</v>
       </c>
     </row>
     <row r="10">
@@ -1016,7 +1016,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>0.954992648469679</v>
+        <v>0.976650822576724</v>
       </c>
     </row>
   </sheetData>
@@ -1063,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.946905309469053</v>
+        <v>0.947405259474053</v>
       </c>
     </row>
     <row r="4">
@@ -1096,7 +1096,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.689431056894311</v>
+        <v>0.673132686731327</v>
       </c>
     </row>
     <row r="7">
@@ -1107,7 +1107,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.318368163183682</v>
+        <v>0.329167083291671</v>
       </c>
     </row>
     <row r="8">
@@ -1187,7 +1187,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0003999600039996</v>
+        <v>0.0005999400059994</v>
       </c>
     </row>
     <row r="5">
@@ -1209,7 +1209,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0600939906009399</v>
+        <v>0.0585941405859414</v>
       </c>
     </row>
     <row r="7">
@@ -1220,7 +1220,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.292170782921708</v>
+        <v>0.302069793020698</v>
       </c>
     </row>
     <row r="8">
@@ -1289,7 +1289,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.195880411958804</v>
+        <v>0.200979902009799</v>
       </c>
     </row>
     <row r="4">
@@ -1300,7 +1300,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0007999200079992</v>
+        <v>0.0001999800019998</v>
       </c>
     </row>
     <row r="5">
@@ -1311,7 +1311,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.478752124787521</v>
+        <v>0.472652734726527</v>
       </c>
     </row>
     <row r="6">
@@ -1333,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.388561143885611</v>
+        <v>0.37986201379862</v>
       </c>
     </row>
     <row r="8">
@@ -1402,7 +1402,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.916808319168083</v>
+        <v>0.906709329067093</v>
       </c>
     </row>
     <row r="4">
@@ -1424,7 +1424,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0001999800019998</v>
+        <v>0.0000999900009999</v>
       </c>
     </row>
     <row r="6">
@@ -1435,7 +1435,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.255874412558744</v>
+        <v>0.245875412458754</v>
       </c>
     </row>
     <row r="7">
@@ -1446,7 +1446,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.855414458554145</v>
+        <v>0.856514348565144</v>
       </c>
     </row>
     <row r="8">
@@ -1515,7 +1515,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.194980501949805</v>
+        <v>0.188981101889811</v>
       </c>
     </row>
     <row r="4">
@@ -1548,7 +1548,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.526747325267473</v>
+        <v>0.518748125187481</v>
       </c>
     </row>
     <row r="7">
@@ -1559,7 +1559,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.788321167883212</v>
+        <v>0.79002099790021</v>
       </c>
     </row>
     <row r="8">
@@ -1570,7 +1570,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.695630436956304</v>
+        <v>0.6996300369963</v>
       </c>
     </row>
     <row r="9">
@@ -1639,7 +1639,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.783721627837216</v>
+        <v>0.781921807819218</v>
       </c>
     </row>
     <row r="4">
@@ -1672,7 +1672,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.465753424657534</v>
+        <v>0.468853114688531</v>
       </c>
     </row>
     <row r="7">
@@ -1683,7 +1683,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.295770422957704</v>
+        <v>0.302269773022698</v>
       </c>
     </row>
     <row r="8">
@@ -1694,7 +1694,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.674632536746325</v>
+        <v>0.67973202679732</v>
       </c>
     </row>
     <row r="9">
@@ -1763,7 +1763,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.805919408059194</v>
+        <v>0.807419258074193</v>
       </c>
     </row>
     <row r="4">
@@ -1785,7 +1785,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.503049695030497</v>
+        <v>0.508049195080492</v>
       </c>
     </row>
     <row r="6">
@@ -1796,7 +1796,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.935206479352065</v>
+        <v>0.932806719328067</v>
       </c>
     </row>
     <row r="7">
@@ -1807,7 +1807,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.846415358464154</v>
+        <v>0.848315168483152</v>
       </c>
     </row>
     <row r="8">
@@ -1876,7 +1876,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.121687831216878</v>
+        <v>0.120887911208879</v>
       </c>
     </row>
     <row r="4">
@@ -1898,7 +1898,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0001999800019998</v>
+        <v>0.0003999600039996</v>
       </c>
     </row>
     <row r="6">
@@ -1909,7 +1909,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0223977602239776</v>
+        <v>0.0212978702129787</v>
       </c>
     </row>
     <row r="7">
@@ -1920,7 +1920,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.849315068493151</v>
+        <v>0.842115788421158</v>
       </c>
     </row>
     <row r="8">
@@ -1931,7 +1931,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.488151184881512</v>
+        <v>0.485451454854515</v>
       </c>
     </row>
     <row r="9">
@@ -2000,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.610838916108389</v>
+        <v>0.614438556144386</v>
       </c>
     </row>
     <row r="4">
@@ -2011,7 +2011,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0002999700029997</v>
+        <v>0.0000999900009999</v>
       </c>
     </row>
     <row r="5">
@@ -2022,7 +2022,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0077992200779922</v>
+        <v>0.0108989101089891</v>
       </c>
     </row>
     <row r="6">
@@ -2033,7 +2033,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.853914608539146</v>
+        <v>0.859414058594141</v>
       </c>
     </row>
     <row r="7">
@@ -2044,7 +2044,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.352564743525647</v>
+        <v>0.354564543545645</v>
       </c>
     </row>
     <row r="8">
@@ -2055,7 +2055,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.283271672832717</v>
+        <v>0.279172082791721</v>
       </c>
     </row>
     <row r="9">
@@ -2124,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.733826617338266</v>
+        <v>0.739126087391261</v>
       </c>
     </row>
     <row r="4">
@@ -2146,7 +2146,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.004999500049995</v>
+        <v>0.0057994200579942</v>
       </c>
     </row>
     <row r="6">
@@ -2157,7 +2157,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.163983601639836</v>
+        <v>0.163483651634837</v>
       </c>
     </row>
     <row r="7">
@@ -2168,7 +2168,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.581041895810419</v>
+        <v>0.576942305769423</v>
       </c>
     </row>
     <row r="8">
@@ -2237,7 +2237,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0472952704729527</v>
+        <v>0.0435956404359564</v>
       </c>
     </row>
     <row r="4">
@@ -2259,7 +2259,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0006999300069993</v>
+        <v>0.0004999500049995</v>
       </c>
     </row>
     <row r="6">
@@ -2270,7 +2270,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.879212078792121</v>
+        <v>0.877812218778122</v>
       </c>
     </row>
     <row r="7">
@@ -2281,7 +2281,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.994100589941006</v>
+        <v>0.993000699930007</v>
       </c>
     </row>
     <row r="8">

</xml_diff>